<commit_message>
Update site reports and DO plots
</commit_message>
<xml_diff>
--- a/Reports/Equipment_Locations_2021_Final.xlsx
+++ b/Reports/Equipment_Locations_2021_Final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Dropbox\Disconnected Sites\GIS\Equipment Locations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Desktop\Box Sync\Thesis\Chinook Seasonal Floodplain Habitat\GitHub\seasonal-floodplains\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B3078A-FE03-40D6-B491-DD6BADAA8A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FA554C-A2A9-402E-96A4-A09C33680863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{35359E95-7EC6-4412-B358-6147D0DBCB02}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="79">
   <si>
     <t>Unit type</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>JB, IH</t>
+  </si>
+  <si>
+    <t>DO Logger</t>
+  </si>
+  <si>
+    <t>Floral Lane Slough</t>
+  </si>
+  <si>
+    <t>IH</t>
   </si>
 </sst>
 </file>
@@ -629,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A3D056-D4B4-4DD6-8193-8CE275562442}">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,6 +651,7 @@
     <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.453125" customWidth="1"/>
     <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.81640625" customWidth="1"/>
     <col min="11" max="11" width="10.7265625" customWidth="1"/>
     <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
@@ -2589,6 +2599,272 @@
         <v>-121.81735</v>
       </c>
     </row>
+    <row r="57" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C57" s="5">
+        <v>44355</v>
+      </c>
+      <c r="D57" s="6">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4">
+        <v>15</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H57" s="5">
+        <v>44354</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K57" s="4">
+        <v>48.487577999999999</v>
+      </c>
+      <c r="L57" s="4">
+        <v>-121.64880700000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C58" s="5">
+        <v>44355</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4">
+        <v>15</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="5">
+        <v>44356</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K58" s="4">
+        <v>48.480938000000002</v>
+      </c>
+      <c r="L58" s="4">
+        <v>-121.58788199999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C59" s="5">
+        <v>44355</v>
+      </c>
+      <c r="D59" s="6">
+        <v>0</v>
+      </c>
+      <c r="E59" s="4">
+        <v>15</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" s="5">
+        <v>44369</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K59" s="4">
+        <v>48.484699999999997</v>
+      </c>
+      <c r="L59" s="4">
+        <v>-121.61375</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C60" s="5">
+        <v>44389</v>
+      </c>
+      <c r="D60" s="6">
+        <v>0</v>
+      </c>
+      <c r="E60" s="4">
+        <v>15</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="5">
+        <v>44389</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K60" s="4">
+        <v>48.497284999999998</v>
+      </c>
+      <c r="L60" s="4">
+        <v>-121.465881</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C61" s="5">
+        <v>44389</v>
+      </c>
+      <c r="D61" s="6">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4">
+        <v>15</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="5">
+        <v>44391</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" s="4">
+        <v>48.512479999999996</v>
+      </c>
+      <c r="L61" s="4">
+        <v>-121.87991</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C62" s="5">
+        <v>44425</v>
+      </c>
+      <c r="D62" s="6">
+        <v>0</v>
+      </c>
+      <c r="E62" s="4">
+        <v>15</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="5">
+        <v>44426</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="4">
+        <v>48.515706000000002</v>
+      </c>
+      <c r="L62" s="4">
+        <v>-122.136735</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="4">
+        <v>21060313</v>
+      </c>
+      <c r="C63" s="5">
+        <v>44460</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E63" s="4">
+        <v>15</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H63" s="5">
+        <v>44460</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K63" s="4">
+        <v>48.503030000000003</v>
+      </c>
+      <c r="L63" s="4">
+        <v>-121.718829</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L56">
     <sortCondition ref="A1:A56"/>

</xml_diff>